<commit_message>
Added basic facet tab tests
</commit_message>
<xml_diff>
--- a/niem-spreadsheet-qa-tests.xlsx
+++ b/niem-spreadsheet-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-format-spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9C8B4A-2121-4988-8100-BEFE8FF5E8FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6292D3B6-FA9E-43FD-A328-2BD144D7434B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="109">
   <si>
     <t>Add</t>
   </si>
@@ -456,6 +456,61 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C6500"/>
       </font>
@@ -539,61 +594,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -611,27 +611,27 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U38" totalsRowShown="0">
   <autoFilter ref="A1:U38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Spec" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{8EEF10A7-EC82-4A12-A76F-38CD1B6C7FFA}" name="Rules" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{FEDA7E3F-4302-4D99-A9AD-A6A3F5DEC6C2}" name="Valid Example" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{4BA8A3FE-15C6-4624-A51D-C6C0B3DF6785}" name="Invalid Example" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{94CEF194-E094-4623-83CB-55148D6F52DC}" name="Exceptions" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{1297B390-DADD-4677-9B74-B7826B32DBFD}" name="Exception IDs" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{C7D09836-0460-412A-9368-B2EC4A488C1E}" name="Notes" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Add" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Edit" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Delete" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Clear" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Map" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Subset" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Spec" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{8EEF10A7-EC82-4A12-A76F-38CD1B6C7FFA}" name="Rules" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{FEDA7E3F-4302-4D99-A9AD-A6A3F5DEC6C2}" name="Valid Example" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{4BA8A3FE-15C6-4624-A51D-C6C0B3DF6785}" name="Invalid Example" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{94CEF194-E094-4623-83CB-55148D6F52DC}" name="Exceptions" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{1297B390-DADD-4677-9B74-B7826B32DBFD}" name="Exception IDs" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{C7D09836-0460-412A-9368-B2EC4A488C1E}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Add" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Edit" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Delete" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Clear" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Map" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Subset" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -903,10 +903,10 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2312,7 @@
       <c r="V29"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2757,35 +2757,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R39:V1048576 P1:U32">
-    <cfRule type="cellIs" dxfId="8" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P33:U38">
-    <cfRule type="cellIs" dxfId="4" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="30" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="31" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="32" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="33" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R39:V1048576 P1:U38">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>